<commit_message>
updated HCRO Time Standard
</commit_message>
<xml_diff>
--- a/Antonio-Feed/FeedPartsInventory.xlsx
+++ b/Antonio-Feed/FeedPartsInventory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pollak/Documents/GitHub/Front-Page/Antonio-Feed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104CD9F6-29BE-F544-9877-AA77993A5402}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63CAD228-3CAE-1049-8043-F27189BE3C40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41060" yWindow="2900" windowWidth="35840" windowHeight="20560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts At ATA" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="438">
   <si>
     <t>Antenna Inventory</t>
   </si>
@@ -1871,14 +1871,14 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2121,29 +2121,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="16">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="80" t="s">
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="81"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="80" t="s">
+      <c r="I1" s="83"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="81"/>
-      <c r="M1" s="81"/>
-      <c r="N1" s="81"/>
-      <c r="O1" s="81"/>
-      <c r="P1" s="81"/>
-      <c r="Q1" s="82"/>
+      <c r="L1" s="83"/>
+      <c r="M1" s="83"/>
+      <c r="N1" s="83"/>
+      <c r="O1" s="83"/>
+      <c r="P1" s="83"/>
+      <c r="Q1" s="84"/>
     </row>
     <row r="2" spans="1:17" ht="16">
       <c r="A2" s="1" t="s">
@@ -3709,38 +3709,38 @@
       <c r="A58" s="17"/>
     </row>
     <row r="59" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A59" s="83" t="s">
+      <c r="A59" s="85" t="s">
         <v>210</v>
       </c>
-      <c r="B59" s="84"/>
-      <c r="C59" s="84"/>
+      <c r="B59" s="81"/>
+      <c r="C59" s="81"/>
     </row>
     <row r="60" spans="1:6" ht="15.75" customHeight="1">
       <c r="A60" s="23"/>
     </row>
     <row r="61" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A61" s="85" t="s">
+      <c r="A61" s="80" t="s">
         <v>202</v>
       </c>
-      <c r="B61" s="84"/>
-      <c r="C61" s="85" t="s">
+      <c r="B61" s="81"/>
+      <c r="C61" s="80" t="s">
         <v>211</v>
       </c>
-      <c r="D61" s="84"/>
-      <c r="E61" s="84"/>
-      <c r="F61" s="84"/>
+      <c r="D61" s="81"/>
+      <c r="E61" s="81"/>
+      <c r="F61" s="81"/>
     </row>
     <row r="62" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A62" s="85" t="s">
+      <c r="A62" s="80" t="s">
         <v>212</v>
       </c>
-      <c r="B62" s="84"/>
-      <c r="C62" s="85" t="s">
+      <c r="B62" s="81"/>
+      <c r="C62" s="80" t="s">
         <v>213</v>
       </c>
-      <c r="D62" s="84"/>
-      <c r="E62" s="84"/>
-      <c r="F62" s="84"/>
+      <c r="D62" s="81"/>
+      <c r="E62" s="81"/>
+      <c r="F62" s="81"/>
     </row>
     <row r="63" spans="1:6" ht="15.75" customHeight="1"/>
     <row r="64" spans="1:6" ht="15.75" customHeight="1"/>
@@ -4708,7 +4708,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -4719,20 +4719,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="82" t="s">
         <v>214</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="80" t="s">
+      <c r="B1" s="84"/>
+      <c r="C1" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
-      <c r="I1" s="81"/>
-      <c r="J1" s="82"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
+      <c r="J1" s="84"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="26" t="s">
@@ -4791,7 +4791,9 @@
       <c r="B4" s="34" t="s">
         <v>219</v>
       </c>
-      <c r="C4" s="35"/>
+      <c r="C4" s="36" t="s">
+        <v>220</v>
+      </c>
       <c r="D4" s="36" t="s">
         <v>220</v>
       </c>
@@ -4803,10 +4805,12 @@
       </c>
       <c r="G4" s="37"/>
       <c r="H4" s="37"/>
-      <c r="I4" s="36" t="s">
+      <c r="I4" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="36" t="s">
         <v>220</v>
       </c>
-      <c r="J4" s="37"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="33" t="str">
@@ -4816,7 +4820,9 @@
       <c r="B5" s="34" t="s">
         <v>221</v>
       </c>
-      <c r="C5" s="35"/>
+      <c r="C5" s="36" t="s">
+        <v>220</v>
+      </c>
       <c r="D5" s="36" t="s">
         <v>220</v>
       </c>
@@ -4828,10 +4834,12 @@
       </c>
       <c r="G5" s="37"/>
       <c r="H5" s="37"/>
-      <c r="I5" s="36" t="s">
+      <c r="I5" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="36" t="s">
         <v>220</v>
       </c>
-      <c r="J5" s="37"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="33" t="str">
@@ -4906,22 +4914,28 @@
       <c r="B9" s="34" t="s">
         <v>225</v>
       </c>
-      <c r="C9" s="35"/>
+      <c r="C9" s="36" t="s">
+        <v>220</v>
+      </c>
       <c r="D9" s="36" t="s">
         <v>220</v>
       </c>
-      <c r="E9" s="36" t="s">
-        <v>220</v>
+      <c r="E9" s="39" t="s">
+        <v>35</v>
       </c>
       <c r="F9" s="36" t="s">
         <v>220</v>
       </c>
       <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="36" t="s">
+      <c r="H9" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="J9" s="36" t="s">
         <v>220</v>
       </c>
-      <c r="J9" s="37"/>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="33" t="str">
@@ -4948,7 +4962,9 @@
       <c r="B11" s="34" t="s">
         <v>227</v>
       </c>
-      <c r="C11" s="35"/>
+      <c r="C11" s="36" t="s">
+        <v>220</v>
+      </c>
       <c r="D11" s="36" t="s">
         <v>220</v>
       </c>
@@ -4960,8 +4976,8 @@
       </c>
       <c r="G11" s="37"/>
       <c r="H11" s="37"/>
-      <c r="I11" s="36" t="s">
-        <v>220</v>
+      <c r="I11" s="39" t="s">
+        <v>35</v>
       </c>
       <c r="J11" s="42" t="s">
         <v>437</v>
@@ -4975,7 +4991,9 @@
       <c r="B12" s="34" t="s">
         <v>228</v>
       </c>
-      <c r="C12" s="35"/>
+      <c r="C12" s="36" t="s">
+        <v>220</v>
+      </c>
       <c r="D12" s="36" t="s">
         <v>220</v>
       </c>
@@ -4987,10 +5005,12 @@
       </c>
       <c r="G12" s="37"/>
       <c r="H12" s="37"/>
-      <c r="I12" s="36" t="s">
+      <c r="I12" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="J12" s="36" t="s">
         <v>220</v>
       </c>
-      <c r="J12" s="37"/>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="33" t="str">
@@ -5066,22 +5086,26 @@
       <c r="B15" s="34" t="s">
         <v>232</v>
       </c>
-      <c r="C15" s="35"/>
+      <c r="C15" s="36" t="s">
+        <v>220</v>
+      </c>
       <c r="D15" s="36" t="s">
         <v>220</v>
       </c>
-      <c r="E15" s="36" t="s">
-        <v>220</v>
+      <c r="E15" s="39" t="s">
+        <v>35</v>
       </c>
       <c r="F15" s="36" t="s">
         <v>220</v>
       </c>
       <c r="G15" s="37"/>
       <c r="H15" s="37"/>
-      <c r="I15" s="36" t="s">
+      <c r="I15" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="J15" s="36" t="s">
         <v>220</v>
       </c>
-      <c r="J15" s="37"/>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="33" t="str">
@@ -5230,7 +5254,7 @@
   </mergeCells>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" fitToHeight="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd"/>
+  <pageSetup paperSize="9" scale="69" fitToHeight="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd"/>
 </worksheet>
 </file>
 
@@ -6591,6 +6615,7 @@
     <row r="1002" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -7869,6 +7894,7 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -8886,6 +8912,7 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -9788,5 +9815,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated network drawing WAN
</commit_message>
<xml_diff>
--- a/Antonio-Feed/FeedPartsInventory.xlsx
+++ b/Antonio-Feed/FeedPartsInventory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pollak/Documents/GitHub/Front-Page/Antonio-Feed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{052DD102-6D3A-154C-87BC-582FD2A23689}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477F4047-4FB4-3948-BE50-C744D6D2D41D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48340" yWindow="4400" windowWidth="35840" windowHeight="20560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="48340" yWindow="4400" windowWidth="35840" windowHeight="20560" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts At ATA" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="475">
   <si>
     <t>Antenna Inventory</t>
   </si>
@@ -2102,6 +2102,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2124,16 +2134,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2379,27 +2379,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="16">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="106" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="103"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
-      <c r="G1" s="104"/>
-      <c r="H1" s="102" t="s">
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="108"/>
+      <c r="H1" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="103"/>
-      <c r="J1" s="103"/>
-      <c r="K1" s="105"/>
-      <c r="L1" s="106"/>
-      <c r="M1" s="106"/>
-      <c r="N1" s="106"/>
-      <c r="O1" s="106"/>
-      <c r="P1" s="106"/>
-      <c r="Q1" s="106"/>
+      <c r="I1" s="107"/>
+      <c r="J1" s="107"/>
+      <c r="K1" s="109"/>
+      <c r="L1" s="110"/>
+      <c r="M1" s="110"/>
+      <c r="N1" s="110"/>
+      <c r="O1" s="110"/>
+      <c r="P1" s="110"/>
+      <c r="Q1" s="110"/>
     </row>
     <row r="2" spans="1:17" ht="16">
       <c r="A2" s="1" t="s">
@@ -3906,38 +3906,38 @@
       <c r="A58" s="13"/>
     </row>
     <row r="59" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A59" s="107" t="s">
+      <c r="A59" s="111" t="s">
         <v>209</v>
       </c>
-      <c r="B59" s="101"/>
-      <c r="C59" s="101"/>
+      <c r="B59" s="105"/>
+      <c r="C59" s="105"/>
     </row>
     <row r="60" spans="1:6" ht="15.75" customHeight="1">
       <c r="A60" s="18"/>
     </row>
     <row r="61" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A61" s="100" t="s">
+      <c r="A61" s="104" t="s">
         <v>201</v>
       </c>
-      <c r="B61" s="101"/>
-      <c r="C61" s="100" t="s">
+      <c r="B61" s="105"/>
+      <c r="C61" s="104" t="s">
         <v>210</v>
       </c>
-      <c r="D61" s="101"/>
-      <c r="E61" s="101"/>
-      <c r="F61" s="101"/>
+      <c r="D61" s="105"/>
+      <c r="E61" s="105"/>
+      <c r="F61" s="105"/>
     </row>
     <row r="62" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A62" s="100" t="s">
+      <c r="A62" s="104" t="s">
         <v>211</v>
       </c>
-      <c r="B62" s="101"/>
-      <c r="C62" s="100" t="s">
+      <c r="B62" s="105"/>
+      <c r="C62" s="104" t="s">
         <v>212</v>
       </c>
-      <c r="D62" s="101"/>
-      <c r="E62" s="101"/>
-      <c r="F62" s="101"/>
+      <c r="D62" s="105"/>
+      <c r="E62" s="105"/>
+      <c r="F62" s="105"/>
     </row>
     <row r="63" spans="1:6" ht="15.75" customHeight="1"/>
     <row r="64" spans="1:6" ht="15.75" customHeight="1"/>
@@ -4900,8 +4900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F153158-615D-8949-B96E-A7AB2B969FBA}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="A1:K21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -4915,20 +4915,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="106" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="104"/>
-      <c r="C1" s="108" t="s">
+      <c r="B1" s="108"/>
+      <c r="C1" s="112" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="105"/>
-      <c r="H1" s="105"/>
-      <c r="I1" s="105"/>
-      <c r="J1" s="105"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="109"/>
+      <c r="I1" s="109"/>
+      <c r="J1" s="109"/>
       <c r="K1" s="97"/>
     </row>
     <row r="2" spans="1:11" ht="17" thickBot="1">
@@ -4962,7 +4962,7 @@
       <c r="J2" s="23" t="s">
         <v>216</v>
       </c>
-      <c r="K2" s="114" t="s">
+      <c r="K2" s="102" t="s">
         <v>474</v>
       </c>
     </row>
@@ -4977,7 +4977,7 @@
       <c r="C3" s="25"/>
       <c r="D3" s="26"/>
       <c r="E3" s="26"/>
-      <c r="F3" s="113" t="s">
+      <c r="F3" s="101" t="s">
         <v>473</v>
       </c>
       <c r="G3" s="26"/>
@@ -4994,7 +4994,7 @@
       <c r="B4" s="28" t="s">
         <v>218</v>
       </c>
-      <c r="C4" s="113" t="s">
+      <c r="C4" s="101" t="s">
         <v>473</v>
       </c>
       <c r="D4" s="33" t="s">
@@ -5015,7 +5015,7 @@
       <c r="I4" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="J4" s="113" t="s">
+      <c r="J4" s="101" t="s">
         <v>473</v>
       </c>
       <c r="K4" s="92"/>
@@ -5116,7 +5116,7 @@
       <c r="C8" s="29"/>
       <c r="D8" s="38"/>
       <c r="E8" s="38"/>
-      <c r="F8" s="113" t="s">
+      <c r="F8" s="101" t="s">
         <v>473</v>
       </c>
       <c r="G8" s="38"/>
@@ -5132,7 +5132,7 @@
       <c r="B9" s="28" t="s">
         <v>223</v>
       </c>
-      <c r="C9" s="113" t="s">
+      <c r="C9" s="101" t="s">
         <v>473</v>
       </c>
       <c r="D9" s="33" t="s">
@@ -5153,10 +5153,10 @@
       <c r="I9" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="J9" s="113" t="s">
+      <c r="J9" s="101" t="s">
         <v>473</v>
       </c>
-      <c r="K9" s="115">
+      <c r="K9" s="103">
         <v>44198</v>
       </c>
     </row>
@@ -5165,7 +5165,7 @@
         <f>HYPERLINK("https://drive.google.com/drive/folders/1EhIIjKRxAQ858Wo2OYQq3GdqbI2ok5Af","5C4-009")</f>
         <v>5C4-009</v>
       </c>
-      <c r="B10" s="112" t="s">
+      <c r="B10" s="100" t="s">
         <v>217</v>
       </c>
       <c r="C10" s="29"/>
@@ -5192,7 +5192,7 @@
       <c r="B11" s="28" t="s">
         <v>465</v>
       </c>
-      <c r="C11" s="113" t="s">
+      <c r="C11" s="101" t="s">
         <v>473</v>
       </c>
       <c r="D11" s="33" t="s">
@@ -5213,10 +5213,10 @@
       <c r="I11" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="J11" s="113" t="s">
+      <c r="J11" s="101" t="s">
         <v>473</v>
       </c>
-      <c r="K11" s="115">
+      <c r="K11" s="103">
         <v>44198</v>
       </c>
     </row>
@@ -5228,7 +5228,7 @@
       <c r="B12" s="28" t="s">
         <v>226</v>
       </c>
-      <c r="C12" s="113" t="s">
+      <c r="C12" s="101" t="s">
         <v>473</v>
       </c>
       <c r="D12" s="33" t="s">
@@ -5249,7 +5249,7 @@
       <c r="I12" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="J12" s="113" t="s">
+      <c r="J12" s="101" t="s">
         <v>473</v>
       </c>
       <c r="K12" s="92"/>
@@ -5330,7 +5330,7 @@
       <c r="B15" s="28" t="s">
         <v>230</v>
       </c>
-      <c r="C15" s="113" t="s">
+      <c r="C15" s="101" t="s">
         <v>473</v>
       </c>
       <c r="D15" s="33" t="s">
@@ -5351,7 +5351,7 @@
       <c r="I15" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="J15" s="113" t="s">
+      <c r="J15" s="101" t="s">
         <v>473</v>
       </c>
       <c r="K15" s="92"/>
@@ -5361,7 +5361,7 @@
         <f>HYPERLINK("https://drive.google.com/drive/folders/1GhnG5G_BN5lBSXzegcxU-3TuUUTEd6xm","5C4-015")</f>
         <v>5C4-015</v>
       </c>
-      <c r="B16" s="112" t="s">
+      <c r="B16" s="100" t="s">
         <v>217</v>
       </c>
       <c r="C16" s="29"/>
@@ -5371,7 +5371,7 @@
       <c r="E16" s="30" t="s">
         <v>219</v>
       </c>
-      <c r="F16" s="113" t="s">
+      <c r="F16" s="101" t="s">
         <v>473</v>
       </c>
       <c r="G16" s="38"/>
@@ -5384,7 +5384,7 @@
       <c r="A17" s="39" t="s">
         <v>231</v>
       </c>
-      <c r="B17" s="112" t="s">
+      <c r="B17" s="100" t="s">
         <v>217</v>
       </c>
       <c r="C17" s="29"/>
@@ -5408,7 +5408,7 @@
         <f>HYPERLINK("https://drive.google.com/drive/folders/1wcHyiuVUbBeL9ODgyYP-lyy7yM1vMH3u","5C4-017")</f>
         <v>5C4-017</v>
       </c>
-      <c r="B18" s="112" t="s">
+      <c r="B18" s="100" t="s">
         <v>217</v>
       </c>
       <c r="C18" s="29"/>
@@ -5418,7 +5418,7 @@
       <c r="E18" s="30" t="s">
         <v>219</v>
       </c>
-      <c r="F18" s="113" t="s">
+      <c r="F18" s="101" t="s">
         <v>473</v>
       </c>
       <c r="G18" s="38"/>
@@ -5541,8 +5541,8 @@
   </sheetPr>
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J21" sqref="A1:J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -5554,20 +5554,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="106" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="104"/>
-      <c r="C1" s="108" t="s">
+      <c r="B1" s="108"/>
+      <c r="C1" s="112" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="105"/>
-      <c r="H1" s="105"/>
-      <c r="I1" s="105"/>
-      <c r="J1" s="105"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="109"/>
+      <c r="I1" s="109"/>
+      <c r="J1" s="109"/>
       <c r="K1" s="97"/>
     </row>
     <row r="2" spans="1:11" ht="17" thickBot="1">
@@ -5796,7 +5796,7 @@
         <f>HYPERLINK("https://drive.google.com/drive/folders/1EhIIjKRxAQ858Wo2OYQq3GdqbI2ok5Af","5C4-009")</f>
         <v>5C4-009</v>
       </c>
-      <c r="B10" s="112" t="s">
+      <c r="B10" s="100" t="s">
         <v>217</v>
       </c>
       <c r="C10" s="29"/>
@@ -5990,7 +5990,7 @@
         <f>HYPERLINK("https://drive.google.com/drive/folders/1GhnG5G_BN5lBSXzegcxU-3TuUUTEd6xm","5C4-015")</f>
         <v>5C4-015</v>
       </c>
-      <c r="B16" s="112" t="s">
+      <c r="B16" s="100" t="s">
         <v>217</v>
       </c>
       <c r="C16" s="29"/>
@@ -6013,21 +6013,23 @@
       <c r="A17" s="39" t="s">
         <v>231</v>
       </c>
-      <c r="B17" s="112" t="s">
+      <c r="B17" s="100" t="s">
         <v>217</v>
       </c>
       <c r="C17" s="29"/>
-      <c r="D17" s="30" t="s">
+      <c r="D17" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" s="31"/>
+      <c r="H17" s="30" t="s">
         <v>219</v>
       </c>
-      <c r="E17" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="F17" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
       <c r="I17" s="31"/>
       <c r="J17" s="31"/>
       <c r="K17" s="92"/>
@@ -6037,7 +6039,7 @@
         <f>HYPERLINK("https://drive.google.com/drive/folders/1wcHyiuVUbBeL9ODgyYP-lyy7yM1vMH3u","5C4-017")</f>
         <v>5C4-017</v>
       </c>
-      <c r="B18" s="112" t="s">
+      <c r="B18" s="100" t="s">
         <v>217</v>
       </c>
       <c r="C18" s="29"/>
@@ -6177,20 +6179,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17" thickBot="1">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="113" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="109" t="s">
+      <c r="B1" s="114"/>
+      <c r="C1" s="113" t="s">
         <v>449</v>
       </c>
-      <c r="D1" s="111"/>
-      <c r="E1" s="111"/>
-      <c r="F1" s="111"/>
-      <c r="G1" s="111"/>
-      <c r="H1" s="111"/>
-      <c r="I1" s="111"/>
-      <c r="J1" s="110"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+      <c r="J1" s="114"/>
     </row>
     <row r="2" spans="1:10" ht="17" thickBot="1">
       <c r="A2" s="86" t="s">

</xml_diff>